<commit_message>
Adding select2 and clear-reset button
</commit_message>
<xml_diff>
--- a/models/data/01simple.xlsx
+++ b/models/data/01simple.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="73">
   <si>
     <t>what time is it</t>
   </si>
@@ -408,6 +408,27 @@
   </si>
   <si>
     <t>Call everyone off the following: &lt;li&gt;Fire Department&lt;/li&gt; &lt;li&gt; DPS&lt;/li&gt; &lt;li&gt;O&amp;M to have an electrician turn off the alarm &lt;/li&gt; &lt;li&gt;Area Director &amp; Building Manager&lt;/li&gt; &lt;li&gt;Create a work order for HSM&lt;/li&gt; &lt;li&gt; Call Landry &lt;/li&gt; &lt;li&gt; Area if necessary to warn the residents&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Plumbing</t>
+  </si>
+  <si>
+    <t>Water Shutdown</t>
+  </si>
+  <si>
+    <t>Priority B &lt;br&gt; 1 – 8 Hours &lt;br&gt; &lt;li&gt;If &lt;strong&gt;scheduled:&lt;/strong&gt; Inform CSC &lt;/li&gt;&lt;li&gt; If &lt;strong&gt;Emergency shutdown: &lt;/strong&gt; Inform resident off the emergency due to which shutdown was done.</t>
+  </si>
+  <si>
+    <t>Toilet</t>
+  </si>
+  <si>
+    <t>Overflowing</t>
+  </si>
+  <si>
+    <t>&lt;li&gt; &lt;strong&gt;Priority A: &lt;/strong&gt; Page GMT &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Priority B: &lt;/strong&gt;&lt;li&gt;If water is dripping wait until morning&lt;/li&gt;&lt;li&gt; If there is stream of water, page gmts&lt;/li&gt; &lt;/li&gt; </t>
+  </si>
+  <si>
+    <t>Leaking</t>
   </si>
 </sst>
 </file>
@@ -537,10 +558,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1365,24 +1386,103 @@
         <v>4</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>65</v>
+      <c r="H29" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding ability to reset all selects and entered more data into excel
</commit_message>
<xml_diff>
--- a/models/data/01simple.xlsx
+++ b/models/data/01simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="922" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="132">
   <si>
     <t>what time is it</t>
   </si>
@@ -242,7 +242,7 @@
     <t>Life/Fire/Safety</t>
   </si>
   <si>
-    <t>Security Grill </t>
+    <t>Security Grill</t>
   </si>
   <si>
     <t>Priority C &lt;br&gt; 24 hours &lt;br&gt; Wait until morning</t>
@@ -268,6 +268,331 @@
   <si>
     <r>
       <t xml:space="preserve">Ask the student since how long has been smelling off gas ? &lt;br&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Instruct the student to turn off all the appliances, keep away from stove and open all the windows. &lt;br&gt; Has there been too many complaints for the same isse ? &lt;li&gt; &lt;strong&gt;Yes, Major Problem&lt;/strong&gt; Inform DPS to evaluate and evacuate as necessary. Call O&amp;M, Building Manager, and/or building AD. If instructed call the Gas company. &lt;/li&gt; &lt;li&gt; Minor Problem, Wait until morning&lt;/li&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Smoke Detectors</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Activation</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority A &lt;br&gt; 1 hour &lt;br&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Call DPS to evaluate the situation. Based on their input, call GMT.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hallway</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority A &lt;br&gt; 1 hour &lt;br&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Call DPS to evaluate the situation. Based on their input,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">call</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, FMS-O&amp;M.</t>
+    </r>
+  </si>
+  <si>
+    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt; Wait until morning for a gmt to address it.</t>
+  </si>
+  <si>
+    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt; Wait until morning for FMS_O&amp;M to address it.</t>
+  </si>
+  <si>
+    <t>Exit Sign</t>
+  </si>
+  <si>
+    <t>Light Bulb</t>
+  </si>
+  <si>
+    <t>Priority B &lt;br&gt; 1 – 8 Hours &lt;br&gt; Wait until morning</t>
+  </si>
+  <si>
+    <t>Sign</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; 1 - 24 Hours Hours &lt;br&gt; Wait until morning</t>
+  </si>
+  <si>
+    <t>Fire Alarm</t>
+  </si>
+  <si>
+    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt;  Assign FMS_O&amp;M</t>
+  </si>
+  <si>
+    <t>Fire Drill</t>
+  </si>
+  <si>
+    <t>Fire Panel</t>
+  </si>
+  <si>
+    <t>Alarm Sounding</t>
+  </si>
+  <si>
+    <t>Assign it to FMS_O&amp;M</t>
+  </si>
+  <si>
+    <t>Light Flashing</t>
+  </si>
+  <si>
+    <t>Wait until morning</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Call everyone off the following: &lt;li&gt;Fire Department&lt;/li&gt; &lt;li&gt; DPS&lt;/li&gt; &lt;li&gt;O&amp;M to have an electrician turn off the alarm &lt;/li&gt; &lt;li&gt;Area Director &amp; Building Manager&lt;/li&gt; &lt;li&gt;Create a work order for HSM&lt;/li&gt; &lt;li&gt; Call Landry &lt;/li&gt; &lt;li&gt; Area if necessary to warn the residents&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Plumbing</t>
+  </si>
+  <si>
+    <t>Water Shutdown</t>
+  </si>
+  <si>
+    <t>Priority B &lt;br&gt; 1 – 8 Hours &lt;br&gt; &lt;li&gt;If &lt;strong&gt;scheduled:&lt;/strong&gt; Inform CSC &lt;/li&gt;&lt;li&gt; If &lt;strong&gt;Emergency shutdown: &lt;/strong&gt; Inform resident off the emergency due to which shutdown was done.</t>
+  </si>
+  <si>
+    <t>Toilet</t>
+  </si>
+  <si>
+    <t>Overflowing</t>
+  </si>
+  <si>
+    <t>&lt;li&gt; &lt;strong&gt;Priority A: &lt;/strong&gt; Page GMT &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Priority B: &lt;/strong&gt;&lt;li&gt;If water is dripping wait until morning&lt;/li&gt;&lt;li&gt; If there is stream of water, page gmts&lt;/li&gt; &lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Leaking</t>
+  </si>
+  <si>
+    <t>&lt;li&gt; &lt;strong&gt;Priority B:  &lt;/strong&gt; &lt;br&gt;1-8 hours&lt;br&gt; Ask The following questions &lt;li&gt;Is water water running inside the tank&lt;/li&gt;&lt;li&gt; Is There water damage to the building/rooms.&lt;/li&gt;&lt;li&gt;Can anyone slip or fall on the water? &lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Not Flushing</t>
+  </si>
+  <si>
+    <t>&lt;li&gt; &lt;strong&gt;Priority A:  &lt;/strong&gt; &lt;br&gt;1-4 hours&lt;br&gt; Ask The following questions &lt;li&gt;Is water water running inside the tank&lt;/li&gt;&lt;li&gt; Is There water damage to the building/rooms.&lt;/li&gt;&lt;li&gt;Can anyone slip or fall on the water? &lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Clogged</t>
+  </si>
+  <si>
+    <t>&lt;li&gt; &lt;strong&gt;Priority A:  &lt;/strong&gt; &lt;br&gt;Ask can they use other toilet ? &lt;br&gt; &lt;strong&gt;If NOT &lt;/strong&gt; &lt;br&gt; Page a GMT &lt;br&gt; &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Priority B:  &lt;/strong&gt;&lt;br&gt;Ask can they use other toilet ? &lt;br&gt; &lt;strong&gt;If NOT &lt;/strong&gt; &lt;br&gt; Page a GMT &lt;br&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>No water pressure / No Hot or Cold water</t>
+  </si>
+  <si>
+    <t>Apartment</t>
+  </si>
+  <si>
+    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt; Assign it to FMS O&amp;M</t>
+  </si>
+  <si>
+    <t>Pipe Burst</t>
+  </si>
+  <si>
+    <t>Problem with boiler or Hot water Header</t>
+  </si>
+  <si>
+    <t>Faucet Leak</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Dripping</t>
+  </si>
+  <si>
+    <t>Stream of water</t>
+  </si>
+  <si>
+    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt; Page it to HSM GMT on call.</t>
+  </si>
+  <si>
+    <t>Shower or Tub Repairs</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; If Scheduled, Wait until Morning</t>
+  </si>
+  <si>
+    <t>Garbage Disposal</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; Wait until Morning</t>
+  </si>
+  <si>
+    <t>Sink</t>
+  </si>
+  <si>
+    <t>Repair / Replacement</t>
+  </si>
+  <si>
+    <t>Schedule - Wait until morning</t>
+  </si>
+  <si>
+    <t>Appliance</t>
+  </si>
+  <si>
+    <t>Laundry</t>
+  </si>
+  <si>
+    <t>Washer/ Dryer</t>
+  </si>
+  <si>
+    <t>Is Broken</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; 1 -24 hours &lt;br&gt; Wait until next day then call Web Services</t>
+  </si>
+  <si>
+    <t>Ask what exactly is broken, is it not spinning or not drying or machine took the money, are there any clothes inside? &lt;br&gt; Wait until next day and call Web Services</t>
+  </si>
+  <si>
+    <t>Dishwasher</t>
+  </si>
+  <si>
+    <t>Water not draining or not working</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; 1 - 24 Hours Hours &lt;br&gt; Askthe resident to turn it off. &lt;li&gt;Ask What kind of soap is being used?&lt;/li&gt; &lt;br&gt; Wait until morning</t>
+  </si>
+  <si>
+    <t>Other Problem</t>
+  </si>
+  <si>
+    <t>Ask What other problem &lt;br&gt; Ask What kind of soap is being used &lt;br&gt; Wait until Morning</t>
+  </si>
+  <si>
+    <t>Stove</t>
+  </si>
+  <si>
+    <t>Did Pilot Light go out</t>
+  </si>
+  <si>
+    <t>Is there gas smell</t>
+  </si>
+  <si>
+    <t>Ask the following questions &lt;ul&gt;&lt;li&gt;How did the pilot light go out&lt;/li&gt;&lt;li&gt;Is the knob turned on?&lt;/li&gt;&lt;br&gt; Instruct the resident to turn off appliances, keep away from the stove and open all the windows. Wait until morning to assign to area.</t>
+  </si>
+  <si>
+    <t>Refer the FIRE/LIFE/SAFETY chart</t>
+  </si>
+  <si>
+    <t>Priority B &lt;br&gt; 48 hours &lt;br&gt; Wait until morning</t>
+  </si>
+  <si>
+    <t>Refrigerator / freezer</t>
+  </si>
+  <si>
+    <t>Priority B &lt;br&gt; 1-8 hours &lt;br&gt; Wait until morning</t>
+  </si>
+  <si>
+    <t>Carpentry</t>
+  </si>
+  <si>
+    <t>Furniture to be repaired</t>
+  </si>
+  <si>
+    <t>Iron-rod repair</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; 24 hours &lt;br&gt; Scheduled: Wait until morning</t>
+  </si>
+  <si>
+    <t>Window screen replacement</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; 48 hours &lt;br&gt; Wait until morning</t>
+  </si>
+  <si>
+    <t>Window ligh replacement</t>
+  </si>
+  <si>
+    <t>Window frame replacement</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; 48 hours &lt;br&gt; Schedule: Wait until morning</t>
+  </si>
+  <si>
+    <t>Window glass cleanup</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority A &lt;br&gt; 1 hour &lt;br&gt;  Ask the following questions: &lt;ul&gt;&lt;li&gt;How did the glass break?&lt;/li&gt;&lt;li&gt;Where exactly is it located ?&lt;/li&gt; &lt;/ul&gt; C</t>
     </r>
     <r>
       <rPr>
@@ -276,24 +601,25 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Instruct the student to turn off all the appliances, keep away from stove and open all the windows. &lt;br&gt; Has there been too many complaints for the same isse ? &lt;li&gt; &lt;strong&gt;Yes, Major Problem&lt;/strong&gt; Inform DPS to evaluate and evacuate as necessary. Call O&amp;M, Building Manager, and/or building AD. If instructed call the Gas company. &lt;/li&gt; &lt;li&gt; Minor Problem, Wait until morning&lt;/li&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>Smoke Detectors</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Activation</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority A &lt;br&gt; 1 hour &lt;br&gt; </t>
+      <t xml:space="preserve">all BSM call Building Manager to schedule his cleaning crew.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Window glass replacement</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority B &lt;br&gt; 4 hours &lt;br&gt; Ask the following questions: &lt;ul&gt;&lt;li&gt;How did the glass break?&lt;/li&gt;&lt;li&gt;Where exactly is it located ?&lt;/li&gt; &lt;/ul&gt; </t>
     </r>
     <r>
       <rPr>
@@ -302,15 +628,17 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Call DPS to evaluate the situation. Based on their input, call GMT.</t>
-    </r>
-  </si>
-  <si>
-    <t>Hallway</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority A &lt;br&gt; 1 hour &lt;br&gt; </t>
+      <t xml:space="preserve">Call DPS to verify if it is a security issue or vandalism. Ask for extra patrol. Call HSM GMT to board-up only.</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -319,16 +647,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Call DPS to evaluate the situation. Based on their input,</t>
+      <t xml:space="preserve">Wait until morning to inform the area and assigned</t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF3366FF"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve"> a vendor for glass replacement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Closet </t>
     </r>
     <r>
       <rPr>
@@ -337,16 +670,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">call</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">Replace/ Tighten/ Fix the closet rods or wheels</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority C &lt;br&gt; 48 hours &lt;br&gt; </t>
     </r>
     <r>
       <rPr>
@@ -355,80 +684,39 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">, FMS-O&amp;M.</t>
-    </r>
-  </si>
-  <si>
-    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt; Wait until morning for a gmt to address it.</t>
-  </si>
-  <si>
-    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt; Wait until morning for FMS_O&amp;M to address it.</t>
-  </si>
-  <si>
-    <t>Exit Sign</t>
-  </si>
-  <si>
-    <t>Light Bulb</t>
-  </si>
-  <si>
-    <t>Priority B &lt;br&gt; 1 – 8 Hours &lt;br&gt; Wait until morning</t>
-  </si>
-  <si>
-    <t>Sign</t>
-  </si>
-  <si>
-    <t>Priority C &lt;br&gt; 1 - 24 Hours Hours &lt;br&gt; Wait until morning</t>
-  </si>
-  <si>
-    <t>Fire Alarm</t>
-  </si>
-  <si>
-    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt;  Assign FMS_O&amp;M</t>
-  </si>
-  <si>
-    <t>Fire Drill</t>
-  </si>
-  <si>
-    <t>Fire Panel</t>
-  </si>
-  <si>
-    <t>Alarm Sounding</t>
-  </si>
-  <si>
-    <t>Assign it to FMS_O&amp;M</t>
-  </si>
-  <si>
-    <t>Light Flashing </t>
-  </si>
-  <si>
-    <t>Wait until morning</t>
-  </si>
-  <si>
-    <t>Fire</t>
-  </si>
-  <si>
-    <t>Call everyone off the following: &lt;li&gt;Fire Department&lt;/li&gt; &lt;li&gt; DPS&lt;/li&gt; &lt;li&gt;O&amp;M to have an electrician turn off the alarm &lt;/li&gt; &lt;li&gt;Area Director &amp; Building Manager&lt;/li&gt; &lt;li&gt;Create a work order for HSM&lt;/li&gt; &lt;li&gt; Call Landry &lt;/li&gt; &lt;li&gt; Area if necessary to warn the residents&lt;/li&gt;</t>
-  </si>
-  <si>
-    <t>Plumbing</t>
-  </si>
-  <si>
-    <t>Water Shutdown</t>
-  </si>
-  <si>
-    <t>Priority B &lt;br&gt; 1 – 8 Hours &lt;br&gt; &lt;li&gt;If &lt;strong&gt;scheduled:&lt;/strong&gt; Inform CSC &lt;/li&gt;&lt;li&gt; If &lt;strong&gt;Emergency shutdown: &lt;/strong&gt; Inform resident off the emergency due to which shutdown was done.</t>
-  </si>
-  <si>
-    <t>Toilet</t>
-  </si>
-  <si>
-    <t>Overflowing</t>
-  </si>
-  <si>
-    <t>&lt;li&gt; &lt;strong&gt;Priority A: &lt;/strong&gt; Page GMT &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Priority B: &lt;/strong&gt;&lt;li&gt;If water is dripping wait until morning&lt;/li&gt;&lt;li&gt; If there is stream of water, page gmts&lt;/li&gt; &lt;/li&gt; </t>
-  </si>
-  <si>
-    <t>Leaking</t>
+      <t xml:space="preserve">Wait until AM, then assign to area. If area sends it back, reassign to GMT or vendor.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Drawer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replace/ Tighten/ Fix the loose drawer(s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority C &lt;br&gt; 48 hours &lt;br&gt; Ask the following questions: &lt;ul&gt;&lt;li&gt;How did the drawer break or get loose?&lt;/li&gt;&lt;li&gt;Where exactly is it located ?&lt;/li&gt; &lt;/ul&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Wait until AM, then assign to area. If area sends it back, reassign to GMT or vendor.</t>
+    </r>
+  </si>
+  <si>
+    <t>Front Door repair/replacement</t>
   </si>
 </sst>
 </file>
@@ -438,7 +726,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -470,13 +758,27 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3366FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -523,7 +825,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -533,10 +835,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -558,10 +856,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H62" activeCellId="0" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -571,7 +869,7 @@
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5546558704453"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.5263157894737"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.6234817813765"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="37.0404858299595"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.5748987854251"/>
@@ -1391,7 +1689,7 @@
       <c r="G27" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1449,7 +1747,7 @@
       <c r="I29" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J29" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1481,8 +1779,972 @@
       <c r="I30" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="J30" s="3" t="s">
-        <v>71</v>
+      <c r="J30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="I43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L48" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K49" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K50" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="L51" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Populated more entries into the excel sheet
</commit_message>
<xml_diff>
--- a/models/data/01simple.xlsx
+++ b/models/data/01simple.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="144">
   <si>
     <t>what time is it</t>
   </si>
@@ -600,6 +600,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">all BSM call Building Manager to schedule his cleaning crew.</t>
     </r>
@@ -627,6 +628,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Call DPS to verify if it is a security issue or vandalism. Ask for extra patrol. Call HSM GMT to board-up only.</t>
     </r>
@@ -637,8 +639,103 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wait until morning to inform the area and assigned</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF3366FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> a vendor for glass replacement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Closet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Replace/ Tighten/ Fix the closet rods or wheels</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority C &lt;br&gt; 48 hours &lt;br&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wait until AM, then assign to area. If area sends it back, reassign to GMT or vendor.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Drawer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Replace/ Tighten/ Fix the loose drawer(s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority C &lt;br&gt; 48 hours &lt;br&gt; Ask the following questions: &lt;ul&gt;&lt;li&gt;How did the drawer break or get loose?&lt;/li&gt;&lt;li&gt;Where exactly is it located ?&lt;/li&gt; &lt;/ul&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wait until AM, then assign to area. If area sends it back, reassign to GMT or vendor.</t>
+    </r>
+  </si>
+  <si>
+    <t>Front Door repair/replacement</t>
+  </si>
+  <si>
+    <t>Is it secure</t>
+  </si>
+  <si>
+    <t>Wait until morning and assign Lock/Frame problem</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority A &lt;br&gt; 1 -4 hour &lt;br&gt; Ask the following questions: &lt;li&gt; Is it off track or hinges ?&lt;/li&gt; &lt;li&gt;Is the lock broken? &lt;/li&gt; </t>
     </r>
     <r>
       <rPr>
@@ -647,76 +744,35 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Wait until morning to inform the area and assigned</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF3366FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a vendor for glass replacement</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Closet </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Replace/ Tighten/ Fix the closet rods or wheels</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority C &lt;br&gt; 48 hours &lt;br&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Wait until AM, then assign to area. If area sends it back, reassign to GMT or vendor.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Drawer </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Replace/ Tighten/ Fix the loose drawer(s)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Priority C &lt;br&gt; 48 hours &lt;br&gt; Ask the following questions: &lt;ul&gt;&lt;li&gt;How did the drawer break or get loose?&lt;/li&gt;&lt;li&gt;Where exactly is it located ?&lt;/li&gt; &lt;/ul&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Wait until AM, then assign to area. If area sends it back, reassign to GMT or vendor.</t>
-    </r>
-  </si>
-  <si>
-    <t>Front Door repair/replacement</t>
+      <t xml:space="preserve">Call DPS to determine if it's a security issue or vandalism. Ask for extra patrol. &lt;br&gt; Call FMS O&amp;M to report the problem</t>
+    </r>
+  </si>
+  <si>
+    <t>Roof</t>
+  </si>
+  <si>
+    <t>Damage Prevention</t>
+  </si>
+  <si>
+    <t>It is scheduled, Assign it to area</t>
+  </si>
+  <si>
+    <t>Leak</t>
+  </si>
+  <si>
+    <t>Is it raining? </t>
+  </si>
+  <si>
+    <t>Wait for rain to stop</t>
+  </si>
+  <si>
+    <t>Priority A or B &lt;br&gt; 1- 72 hours &lt;br&gt; Ask the following questions:  &lt;li&gt;Where exactly is the leak&lt;/li&gt; &lt;li&gt;How much water flowing&lt;/li&gt; &lt;li&gt; Is there visible water damange ?&lt;/li&gt;  &lt;br&gt; &lt;li&gt; Is it dripping or stream of water? &lt;/li&gt; &lt;li&gt;If Drip: there another room above? no room above - did it rain the previous day/send to the area to clean the roof.. Instruct the resident to place a bucket to receive the water and wait 'till the AM to send a GMT or FMS &lt;/li&gt; &lt;li&gt;If Stream: &lt;/li&gt;is there another room above, no room above - did it rain the previous day/send to the area to clean the roof. Page gmts to inspect or FMS if GMTs state that they can fix it</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>Need to Wait until morning</t>
   </si>
 </sst>
 </file>
@@ -764,21 +820,23 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF3366FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -856,10 +914,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H62" activeCellId="0" sqref="H62"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G65" activeCellId="0" sqref="G65:J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2744,7 +2802,164 @@
         <v>131</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>6</v>
+        <v>132</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Populated more data into excel
</commit_message>
<xml_diff>
--- a/models/data/01simple.xlsx
+++ b/models/data/01simple.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="187">
   <si>
     <t>what time is it</t>
   </si>
@@ -743,6 +743,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Call DPS to determine if it's a security issue or vandalism. Ask for extra patrol. &lt;br&gt; Call FMS O&amp;M to report the problem</t>
     </r>
@@ -760,7 +761,7 @@
     <t>Leak</t>
   </si>
   <si>
-    <t>Is it raining? </t>
+    <t>Is it raining?</t>
   </si>
   <si>
     <t>Wait for rain to stop</t>
@@ -773,6 +774,178 @@
   </si>
   <si>
     <t>Need to Wait until morning</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Can't Make outgoing calls</t>
+  </si>
+  <si>
+    <t>Priority B &lt;br&gt; 1 – 8 hours &lt;br&gt; Ask the following questions &lt;li&gt;Can you please provide the phone number you are having problems with&lt;/li&gt; &lt;li&gt;Have you tried plugging the phone into another jack ?&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>Can't hear dial tone</t>
+  </si>
+  <si>
+    <t>Can't hear rings</t>
+  </si>
+  <si>
+    <t>Problem calling long distance</t>
+  </si>
+  <si>
+    <t>Notify the resident that USC does not offer long distance calls. She/he may use a calling card.</t>
+  </si>
+  <si>
+    <t>Problem with Second line</t>
+  </si>
+  <si>
+    <t>It is Scheduled. Wait until morning.</t>
+  </si>
+  <si>
+    <t>Building outage</t>
+  </si>
+  <si>
+    <t>Call Manny at home and wait until morning to call ISD. Or do what Manny says.</t>
+  </si>
+  <si>
+    <t>Patch and Paint</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>It is Scheduled, wait until morning</t>
+  </si>
+  <si>
+    <t>There is a hole in the hallway</t>
+  </si>
+  <si>
+    <t>There an graffiti</t>
+  </si>
+  <si>
+    <t>Priority A or B &lt;br&gt; 1 – 8 hours &lt;br&gt; Ask the following questions &lt;li&gt;Where exactly is the graffiti?&lt;/li&gt;&lt;li&gt;Is the wording offensive or can cause an outrage?&lt;/li&gt; &lt;br&gt; Call the area on call technician depending on the severity and the location. Else wait till morning</t>
+  </si>
+  <si>
+    <t>Landscape</t>
+  </si>
+  <si>
+    <t>Is the sprinkler broken?</t>
+  </si>
+  <si>
+    <t>Priority A or B &lt;br&gt; 1- 8 hours &lt;br&gt; Ask the following questions &lt;li&gt;Is the water  spilling onto the sidewalk? &lt;/li&gt;&lt;li&gt;Can someone split and get hurt?&lt;/li&gt;&lt;li&gt;Is there a flood?&lt;/li&gt; &lt;br&gt; </t>
+  </si>
+  <si>
+    <t>Trim/ remove trees/plants</t>
+  </si>
+  <si>
+    <t>Priority C &lt;br&gt; 5 days &lt;br&gt; Wait until Morning</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Auto gate</t>
+  </si>
+  <si>
+    <t>Is it not making a sounds?</t>
+  </si>
+  <si>
+    <t>Priority A &lt;br&gt; 1 - 4 hours &lt;br&gt; The motor is probably not working &lt;br&gt; Ask the following questions: &lt;ul&gt;&lt;li&gt;The door in open or closed position&lt;/li&gt;&lt;li&gt;What happens when you swipe the card?&lt;/li&gt;&lt;li&gt;If there is not light, did you try replacing the batteries&lt;/li&gt; &lt;/ul&gt; After hours autogates call DPS and if problem is not resolve by DPS ask them to patol and call Transportation Services in the morning or Pablo's office at 213-743-1738 &lt;strong&gt;Transportation Services: 08709&lt;/strong&gt;&lt;strong&gt;Call DPS and ask them for security around that area.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Is it not opening</t>
+  </si>
+  <si>
+    <t>If stuck in a closed position: Priority A &lt;br&gt; 1 – 4 hours &lt;br&gt; What is the exact building and location of the gate? &lt;br&gt; Use the autogate flowchart from the desk handbook for autogate number. &lt;br&gt; After hours autogates call DPS and if problem is not resolve by DPS ask them to patol and call Transportation Services in the morning or Pablo's office at 213-743-1738 &lt;strong&gt;Transportation Services: 08709&lt;/strong&gt;&lt;strong&gt;Call DPS and ask them for security around that area.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Is it not closing</t>
+  </si>
+  <si>
+    <t>Priority A &lt;br&gt; 1 – 8 hours &lt;br&gt; &lt;li&gt;Is it partially or completely open&lt;/li&gt; &lt;li&gt; What is the exact building and location of the gate? &lt;/li&gt; &lt;br&gt; Use the autogate flowchart from the desk handbook for autogate number. &lt;br&gt; After hours autogates call DPS and if problem is not resolve by DPS ask them to patol and call Transportation Services in the morning or Pablo's office at 213-743-1738 &lt;strong&gt;Transportation Services: 08709&lt;/strong&gt;&lt;strong&gt;Call DPS and ask them for security around that area.&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Access card</t>
+  </si>
+  <si>
+    <t>Mode of card when swiped</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Priority A or B &lt;br&gt; 1 – 4 hours &lt;br&gt; If it is not releasing or is broken, the door magnet is not working. &lt;br&gt; Do the following:  &lt;li&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Call RA on duty and ask them to let the student into his/her appartment.&lt;/li&gt;&lt;li&gt;Call DPS to patrol the area more frequently.&lt;/li&gt;&lt;li&gt;In the morning: Contact USCard (08709)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/li&gt; </t>
+    </r>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Priority A or B &lt;br&gt; 1 – 4 hours &lt;br&gt; If it is not reading or releasing, it is a card reader problem. &lt;br&gt; Do the following:  &lt;li&gt; Call RA on duty and ask them to let the student into his/her appartment.&lt;/li&gt;&lt;li&gt;Call DPS to patrol the area more frequently.&lt;/li&gt;&lt;li&gt;In the morning: Contact USCard (08709)&lt;/li&gt;&lt;br&gt; </t>
+  </si>
+  <si>
+    <t>Custodial</t>
+  </si>
+  <si>
+    <t>Shampoo rugs / rugs need cleaning</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scheduled &lt;br&gt; Ask the follow: &lt;li&gt;Why does your rug need cleanning?&lt;/li&gt; Inform </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Area on call technician depending on severity &amp; location. Otherwise, wait until morning.</t>
+    </r>
+  </si>
+  <si>
+    <t>Move or replace furniture</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scheduled, Inform </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Area on call technician depending on severity &amp; location. Otherwise, wait until morning.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -782,7 +955,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -840,6 +1013,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -883,7 +1062,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -893,6 +1072,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,10 +1097,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G65" activeCellId="0" sqref="G65:J66"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H88" activeCellId="0" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2962,6 +3145,526 @@
         <v>143</v>
       </c>
     </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H70" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H76" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H84" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F86" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H86" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F87" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added more data to excel to populate it, move index.html for simpler URL, modified main.js
</commit_message>
<xml_diff>
--- a/models/data/01simple.xlsx
+++ b/models/data/01simple.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="193">
   <si>
     <t>what time is it</t>
   </si>
@@ -462,19 +462,19 @@
     <t>Overflowing</t>
   </si>
   <si>
-    <t>&lt;li&gt; &lt;strong&gt;Priority A: &lt;/strong&gt; Page GMT &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Priority B: &lt;/strong&gt;&lt;li&gt;If water is dripping wait until morning&lt;/li&gt;&lt;li&gt; If there is stream of water, page gmts&lt;/li&gt; &lt;/li&gt;</t>
+    <t>&lt;li&gt; &lt;strong&gt;Priority A: &lt;/strong&gt; Page GMT &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Priority B: &lt;/strong&gt;&lt;li&gt;If water is dripping wait until morning&lt;/li&gt;&lt;li&gt; If there is stream of water, page gmts&lt;/li&gt; &lt;/li&gt; &lt;li&gt;If clean up is required, call BSM to coordinate&lt;/li&gt;</t>
   </si>
   <si>
     <t>Leaking</t>
   </si>
   <si>
-    <t>&lt;li&gt; &lt;strong&gt;Priority B:  &lt;/strong&gt; &lt;br&gt;1-8 hours&lt;br&gt; Ask The following questions &lt;li&gt;Is water water running inside the tank&lt;/li&gt;&lt;li&gt; Is There water damage to the building/rooms.&lt;/li&gt;&lt;li&gt;Can anyone slip or fall on the water? &lt;/li&gt;</t>
+    <t>&lt;li&gt; &lt;strong&gt;Priority B:  &lt;/strong&gt; &lt;br&gt;1-8 hours&lt;br&gt; Ask The following questions &lt;li&gt;Is water water running inside the tank&lt;/li&gt;&lt;li&gt; Is There water damage to the building/rooms.&lt;/li&gt;&lt;li&gt;Can anyone slip or fall on the water? &lt;/li&gt; &lt;If there is water damage, call GMT &lt;/li&gt;</t>
   </si>
   <si>
     <t>Not Flushing</t>
   </si>
   <si>
-    <t>&lt;li&gt; &lt;strong&gt;Priority A:  &lt;/strong&gt; &lt;br&gt;1-4 hours&lt;br&gt; Ask The following questions &lt;li&gt;Is water water running inside the tank&lt;/li&gt;&lt;li&gt; Is There water damage to the building/rooms.&lt;/li&gt;&lt;li&gt;Can anyone slip or fall on the water? &lt;/li&gt;</t>
+    <t>&lt;li&gt; &lt;strong&gt;Priority A:  &lt;/strong&gt; &lt;br&gt;1-4 hours&lt;br&gt; Ask The following questions &lt;li&gt;Is water water running inside the tank&lt;/li&gt;&lt;li&gt; Is There water damage to the building/rooms.&lt;/li&gt;&lt;li&gt;Can anyone slip or fall on the water? &lt;/li&gt; &lt; Ask, if there is any other toilet they can use &lt;/li&gt;</t>
   </si>
   <si>
     <t>Clogged</t>
@@ -495,6 +495,9 @@
     <t>Pipe Burst</t>
   </si>
   <si>
+    <t>Priority A &lt;br&gt; 1 hour &lt;br&gt;  Assign FMS_O&amp;M &lt;br&gt; Follow up with FMS, after half (½) an hour</t>
+  </si>
+  <si>
     <t>Problem with boiler or Hot water Header</t>
   </si>
   <si>
@@ -528,6 +531,9 @@
     <t>Sink</t>
   </si>
   <si>
+    <t>Priority C &lt;br&gt; 1 - 24 Hours Hours &lt;br&gt; Wait until morning, unless it is overflowing</t>
+  </si>
+  <si>
     <t>Repair / Replacement</t>
   </si>
   <si>
@@ -549,7 +555,7 @@
     <t>Priority C &lt;br&gt; 1 -24 hours &lt;br&gt; Wait until next day then call Web Services</t>
   </si>
   <si>
-    <t>Ask what exactly is broken, is it not spinning or not drying or machine took the money, are there any clothes inside? &lt;br&gt; Wait until next day and call Web Services</t>
+    <t>Ask what exactly is broken, is it not spinning or not drying or machine took the money, are there any clothes inside? &lt;br&gt; Wait until next day and call Web Services &lt;br&gt; If there is a severe leak, call wash services, they are 24/7</t>
   </si>
   <si>
     <t>Dishwasher</t>
@@ -577,6 +583,9 @@
   </si>
   <si>
     <t>Ask the following questions &lt;ul&gt;&lt;li&gt;How did the pilot light go out&lt;/li&gt;&lt;li&gt;Is the knob turned on?&lt;/li&gt;&lt;br&gt; Instruct the resident to turn off appliances, keep away from the stove and open all the windows. Wait until morning to assign to area.</t>
+  </si>
+  <si>
+    <t>&lt;li&gt; Refer the FIRE/LIFE/SAFETY chart &lt;/li&gt; &lt;li&gt;Page the GMT on call&lt;/li&gt;&lt;li&gt;Request windows to be opened &lt;/li&gt;</t>
   </si>
   <si>
     <t>Refer the FIRE/LIFE/SAFETY chart</t>
@@ -836,7 +845,7 @@
     <t>Building outage</t>
   </si>
   <si>
-    <t>Call Manny at home and wait until morning to call ISD. Or do what Manny says.</t>
+    <t>Call Manny at home and wait until morning to call ISD. Or do what Manny says. &lt;br&gt; Also call ITS after hours</t>
   </si>
   <si>
     <t>Patch and Paint</t>
@@ -863,7 +872,7 @@
     <t>Is the sprinkler broken?</t>
   </si>
   <si>
-    <t>Priority A or B &lt;br&gt; 1- 8 hours &lt;br&gt; Ask the following questions &lt;li&gt;Is the water  spilling onto the sidewalk? &lt;/li&gt;&lt;li&gt;Can someone split and get hurt?&lt;/li&gt;&lt;li&gt;Is there a flood?&lt;/li&gt; &lt;br&gt;</t>
+    <t>Priority A or B &lt;br&gt; 1- 8 hours &lt;br&gt; Ask the following questions &lt;li&gt;Is the water  spilling onto the sidewalk? &lt;/li&gt;&lt;li&gt;Can someone split and get hurt?&lt;/li&gt;&lt;li&gt;Is there a flood?&lt;/li&gt; &lt;br&gt; Assign it to FMS</t>
   </si>
   <si>
     <t>Trim/ remove trees/plants</t>
@@ -876,6 +885,9 @@
   </si>
   <si>
     <t>repair</t>
+  </si>
+  <si>
+    <t>Wait until morning, then assign it to the area to handle</t>
   </si>
   <si>
     <t>Cleaning</t>
@@ -959,7 +971,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Area on call technician depending on severity &amp; location. Otherwise, wait until morning.</t>
+      <t xml:space="preserve">Area on call technician depending on severity &amp; location. Request, BSM to coordinate, if the need to come after hours. Otherwise, wait until morning.</t>
     </r>
   </si>
   <si>
@@ -977,7 +989,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Area on call technician depending on severity &amp; location. Otherwise, wait until morning.</t>
+      <t xml:space="preserve">Area on call technician depending on severity &amp; location. Request BMS to coordinate if they need to come after hours. Otherwise, wait until morning.</t>
     </r>
   </si>
 </sst>
@@ -1130,8 +1142,8 @@
   </sheetPr>
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E62" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H88" activeCellId="0" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2290,7 +2302,7 @@
         <v>6</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="I35" s="0"/>
       <c r="J35" s="0"/>
@@ -2314,7 +2326,7 @@
         <v>4</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>6</v>
@@ -2344,13 +2356,13 @@
         <v>4</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>6</v>
@@ -2378,19 +2390,19 @@
         <v>4</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K38" s="0"/>
       <c r="L38" s="0"/>
@@ -2412,13 +2424,13 @@
         <v>4</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I39" s="0"/>
       <c r="J39" s="0"/>
@@ -2442,13 +2454,13 @@
         <v>4</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I40" s="0"/>
       <c r="J40" s="0"/>
@@ -2472,7 +2484,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>45</v>
@@ -2506,7 +2518,7 @@
         <v>4</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>45</v>
@@ -2518,7 +2530,7 @@
         <v>6</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
       <c r="K42" s="0"/>
       <c r="L42" s="0"/>
@@ -2540,19 +2552,19 @@
         <v>4</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K43" s="0"/>
       <c r="L43" s="0"/>
@@ -2568,22 +2580,22 @@
         <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>14</v>
@@ -2592,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,22 +2618,22 @@
         <v>2</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>16</v>
@@ -2630,7 +2642,7 @@
         <v>6</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2644,25 +2656,25 @@
         <v>2</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K46" s="0"/>
       <c r="L46" s="0"/>
@@ -2678,25 +2690,25 @@
         <v>2</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K47" s="0"/>
       <c r="L47" s="0"/>
@@ -2712,22 +2724,22 @@
         <v>2</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>16</v>
@@ -2736,7 +2748,7 @@
         <v>6</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,22 +2762,22 @@
         <v>2</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>14</v>
@@ -2774,7 +2786,7 @@
         <v>6</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,22 +2800,22 @@
         <v>2</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>14</v>
@@ -2812,7 +2824,7 @@
         <v>6</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,22 +2838,22 @@
         <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>16</v>
@@ -2850,7 +2862,7 @@
         <v>6</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2864,13 +2876,13 @@
         <v>2</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>6</v>
@@ -2892,13 +2904,13 @@
         <v>2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>6</v>
@@ -2920,19 +2932,19 @@
         <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="I54" s="0"/>
       <c r="J54" s="0"/>
@@ -2948,19 +2960,19 @@
         <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I55" s="0"/>
       <c r="J55" s="0"/>
@@ -2976,17 +2988,17 @@
         <v>2</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G56" s="0"/>
       <c r="H56" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I56" s="0"/>
       <c r="J56" s="0"/>
@@ -3002,19 +3014,19 @@
         <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="I57" s="0"/>
       <c r="J57" s="0"/>
@@ -3030,19 +3042,19 @@
         <v>2</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="I58" s="0"/>
       <c r="J58" s="0"/>
@@ -3058,19 +3070,19 @@
         <v>2</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="I59" s="0"/>
       <c r="J59" s="0"/>
@@ -3086,19 +3098,19 @@
         <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="I60" s="0"/>
       <c r="J60" s="0"/>
@@ -3114,19 +3126,19 @@
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I61" s="0"/>
       <c r="J61" s="0"/>
@@ -3142,16 +3154,16 @@
         <v>2</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>14</v>
@@ -3160,7 +3172,7 @@
         <v>6</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,16 +3186,16 @@
         <v>2</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>16</v>
@@ -3192,7 +3204,7 @@
         <v>6</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3206,19 +3218,19 @@
         <v>2</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I64" s="0"/>
       <c r="J64" s="0"/>
@@ -3234,16 +3246,16 @@
         <v>2</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>14</v>
@@ -3252,7 +3264,7 @@
         <v>6</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,16 +3278,16 @@
         <v>2</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>16</v>
@@ -3284,7 +3296,7 @@
         <v>6</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3298,19 +3310,19 @@
         <v>2</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3324,19 +3336,19 @@
         <v>2</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3350,19 +3362,19 @@
         <v>2</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3376,19 +3388,19 @@
         <v>2</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,19 +3414,19 @@
         <v>2</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3428,19 +3440,19 @@
         <v>2</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3454,19 +3466,19 @@
         <v>2</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3480,19 +3492,19 @@
         <v>2</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3506,13 +3518,13 @@
         <v>2</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>6</v>
@@ -3532,19 +3544,19 @@
         <v>2</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3558,19 +3570,19 @@
         <v>2</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3584,19 +3596,19 @@
         <v>2</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G78" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,19 +3622,19 @@
         <v>2</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3636,19 +3648,19 @@
         <v>2</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3662,19 +3674,19 @@
         <v>2</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,19 +3700,19 @@
         <v>2</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,19 +3726,19 @@
         <v>2</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,19 +3752,19 @@
         <v>2</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3766,19 +3778,19 @@
         <v>2</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3792,19 +3804,19 @@
         <v>2</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,19 +3830,19 @@
         <v>2</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>